<commit_message>
Beginning of reconfigure for backend
</commit_message>
<xml_diff>
--- a/compiled.xlsx
+++ b/compiled.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ULB Info" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="Services" sheetId="6" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ULB Info'!$A$1:$F$111</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="168">
   <si>
     <t>ANANTAPUR</t>
   </si>
@@ -451,18 +454,6 @@
   </si>
   <si>
     <t>Timeliness</t>
-  </si>
-  <si>
-    <t>PGR Accuracy</t>
-  </si>
-  <si>
-    <t>Property Tax Accuracy</t>
-  </si>
-  <si>
-    <t>Water Tax Accuracy</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
   </si>
   <si>
     <t>Functionary</t>
@@ -898,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3131,16 +3122,17 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F111"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3149,13 +3141,10 @@
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -3171,20 +3160,8 @@
       <c r="E1" t="s">
         <v>138</v>
       </c>
-      <c r="F1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -3200,20 +3177,8 @@
       <c r="E2">
         <v>0.40830917900000002</v>
       </c>
-      <c r="F2">
-        <v>0.5</v>
-      </c>
-      <c r="G2">
-        <v>0.5</v>
-      </c>
-      <c r="H2">
-        <v>0.5</v>
-      </c>
-      <c r="I2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -3229,20 +3194,8 @@
       <c r="E3">
         <v>0.51890212300000005</v>
       </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-      <c r="G3">
-        <v>0.5</v>
-      </c>
-      <c r="H3">
-        <v>0.5</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -3258,20 +3211,8 @@
       <c r="E4">
         <v>0.50033760999999999</v>
       </c>
-      <c r="F4">
-        <v>0.5</v>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -3287,20 +3228,8 @@
       <c r="E5">
         <v>0.55522136700000002</v>
       </c>
-      <c r="F5">
-        <v>0.5</v>
-      </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
-      <c r="H5">
-        <v>0.5</v>
-      </c>
-      <c r="I5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -3316,20 +3245,8 @@
       <c r="E6">
         <v>0.56713476200000001</v>
       </c>
-      <c r="F6">
-        <v>0.5</v>
-      </c>
-      <c r="G6">
-        <v>0.5</v>
-      </c>
-      <c r="H6">
-        <v>0.5</v>
-      </c>
-      <c r="I6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -3345,20 +3262,8 @@
       <c r="E7">
         <v>0.60034802799999998</v>
       </c>
-      <c r="F7">
-        <v>0.5</v>
-      </c>
-      <c r="G7">
-        <v>0.5</v>
-      </c>
-      <c r="H7">
-        <v>0.5</v>
-      </c>
-      <c r="I7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -3374,20 +3279,8 @@
       <c r="E8">
         <v>0.67366015800000001</v>
       </c>
-      <c r="F8">
-        <v>0.5</v>
-      </c>
-      <c r="G8">
-        <v>0.5</v>
-      </c>
-      <c r="H8">
-        <v>0.5</v>
-      </c>
-      <c r="I8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -3403,20 +3296,8 @@
       <c r="E9">
         <v>0.66124661200000001</v>
       </c>
-      <c r="F9">
-        <v>0.5</v>
-      </c>
-      <c r="G9">
-        <v>0.5</v>
-      </c>
-      <c r="H9">
-        <v>0.5</v>
-      </c>
-      <c r="I9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -3432,20 +3313,8 @@
       <c r="E10">
         <v>0.47890499199999997</v>
       </c>
-      <c r="F10">
-        <v>0.5</v>
-      </c>
-      <c r="G10">
-        <v>0.5</v>
-      </c>
-      <c r="H10">
-        <v>0.5</v>
-      </c>
-      <c r="I10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1010</v>
       </c>
@@ -3461,20 +3330,8 @@
       <c r="E11">
         <v>0.53092569499999998</v>
       </c>
-      <c r="F11">
-        <v>0.5</v>
-      </c>
-      <c r="G11">
-        <v>0.5</v>
-      </c>
-      <c r="H11">
-        <v>0.5</v>
-      </c>
-      <c r="I11">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -3490,20 +3347,8 @@
       <c r="E12">
         <v>0.41511500499999998</v>
       </c>
-      <c r="F12">
-        <v>0.5</v>
-      </c>
-      <c r="G12">
-        <v>0.5</v>
-      </c>
-      <c r="H12">
-        <v>0.5</v>
-      </c>
-      <c r="I12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1012</v>
       </c>
@@ -3519,20 +3364,8 @@
       <c r="E13">
         <v>0.52268395000000001</v>
       </c>
-      <c r="F13">
-        <v>0.5</v>
-      </c>
-      <c r="G13">
-        <v>0.5</v>
-      </c>
-      <c r="H13">
-        <v>0.5</v>
-      </c>
-      <c r="I13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1013</v>
       </c>
@@ -3548,20 +3381,8 @@
       <c r="E14">
         <v>0.45865513299999999</v>
       </c>
-      <c r="F14">
-        <v>0.5</v>
-      </c>
-      <c r="G14">
-        <v>0.5</v>
-      </c>
-      <c r="H14">
-        <v>0.5</v>
-      </c>
-      <c r="I14">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1014</v>
       </c>
@@ -3577,20 +3398,8 @@
       <c r="E15">
         <v>0.35869799499999999</v>
       </c>
-      <c r="F15">
-        <v>0.5</v>
-      </c>
-      <c r="G15">
-        <v>0.5</v>
-      </c>
-      <c r="H15">
-        <v>0.5</v>
-      </c>
-      <c r="I15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1015</v>
       </c>
@@ -3606,20 +3415,8 @@
       <c r="E16">
         <v>0.48585572799999999</v>
       </c>
-      <c r="F16">
-        <v>0.5</v>
-      </c>
-      <c r="G16">
-        <v>0.5</v>
-      </c>
-      <c r="H16">
-        <v>0.5</v>
-      </c>
-      <c r="I16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1016</v>
       </c>
@@ -3635,20 +3432,8 @@
       <c r="E17">
         <v>0.47805847600000001</v>
       </c>
-      <c r="F17">
-        <v>0.5</v>
-      </c>
-      <c r="G17">
-        <v>0.5</v>
-      </c>
-      <c r="H17">
-        <v>0.5</v>
-      </c>
-      <c r="I17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1017</v>
       </c>
@@ -3664,20 +3449,8 @@
       <c r="E18">
         <v>0.41809653099999999</v>
       </c>
-      <c r="F18">
-        <v>0.5</v>
-      </c>
-      <c r="G18">
-        <v>0.5</v>
-      </c>
-      <c r="H18">
-        <v>0.5</v>
-      </c>
-      <c r="I18">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1018</v>
       </c>
@@ -3693,20 +3466,8 @@
       <c r="E19">
         <v>0.57580346599999999</v>
       </c>
-      <c r="F19">
-        <v>0.5</v>
-      </c>
-      <c r="G19">
-        <v>0.5</v>
-      </c>
-      <c r="H19">
-        <v>0.5</v>
-      </c>
-      <c r="I19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1019</v>
       </c>
@@ -3722,20 +3483,8 @@
       <c r="E20">
         <v>0.44397217900000002</v>
       </c>
-      <c r="F20">
-        <v>0.5</v>
-      </c>
-      <c r="G20">
-        <v>0.5</v>
-      </c>
-      <c r="H20">
-        <v>0.5</v>
-      </c>
-      <c r="I20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1020</v>
       </c>
@@ -3751,20 +3500,8 @@
       <c r="E21">
         <v>0.63133208299999999</v>
       </c>
-      <c r="F21">
-        <v>0.5</v>
-      </c>
-      <c r="G21">
-        <v>0.5</v>
-      </c>
-      <c r="H21">
-        <v>0.5</v>
-      </c>
-      <c r="I21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1021</v>
       </c>
@@ -3780,20 +3517,8 @@
       <c r="E22">
         <v>0.40652048000000002</v>
       </c>
-      <c r="F22">
-        <v>0.5</v>
-      </c>
-      <c r="G22">
-        <v>0.5</v>
-      </c>
-      <c r="H22">
-        <v>0.5</v>
-      </c>
-      <c r="I22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1022</v>
       </c>
@@ -3809,20 +3534,8 @@
       <c r="E23">
         <v>0.58061785899999996</v>
       </c>
-      <c r="F23">
-        <v>0.5</v>
-      </c>
-      <c r="G23">
-        <v>0.5</v>
-      </c>
-      <c r="H23">
-        <v>0.5</v>
-      </c>
-      <c r="I23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1023</v>
       </c>
@@ -3838,20 +3551,8 @@
       <c r="E24">
         <v>0.34993614299999998</v>
       </c>
-      <c r="F24">
-        <v>0.5</v>
-      </c>
-      <c r="G24">
-        <v>0.5</v>
-      </c>
-      <c r="H24">
-        <v>0.5</v>
-      </c>
-      <c r="I24">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1024</v>
       </c>
@@ -3867,20 +3568,8 @@
       <c r="E25">
         <v>0.57623661400000004</v>
       </c>
-      <c r="F25">
-        <v>0.5</v>
-      </c>
-      <c r="G25">
-        <v>0.5</v>
-      </c>
-      <c r="H25">
-        <v>0.5</v>
-      </c>
-      <c r="I25">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1025</v>
       </c>
@@ -3896,20 +3585,8 @@
       <c r="E26">
         <v>0.54166666699999999</v>
       </c>
-      <c r="F26">
-        <v>0.5</v>
-      </c>
-      <c r="G26">
-        <v>0.5</v>
-      </c>
-      <c r="H26">
-        <v>0.5</v>
-      </c>
-      <c r="I26">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1026</v>
       </c>
@@ -3925,20 +3602,8 @@
       <c r="E27">
         <v>0.48444599799999999</v>
       </c>
-      <c r="F27">
-        <v>0.5</v>
-      </c>
-      <c r="G27">
-        <v>0.5</v>
-      </c>
-      <c r="H27">
-        <v>0.5</v>
-      </c>
-      <c r="I27">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1027</v>
       </c>
@@ -3954,20 +3619,8 @@
       <c r="E28">
         <v>0.42297047999999998</v>
       </c>
-      <c r="F28">
-        <v>0.5</v>
-      </c>
-      <c r="G28">
-        <v>0.5</v>
-      </c>
-      <c r="H28">
-        <v>0.5</v>
-      </c>
-      <c r="I28">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1028</v>
       </c>
@@ -3983,20 +3636,8 @@
       <c r="E29">
         <v>0.36433421900000001</v>
       </c>
-      <c r="F29">
-        <v>0.5</v>
-      </c>
-      <c r="G29">
-        <v>0.5</v>
-      </c>
-      <c r="H29">
-        <v>0.5</v>
-      </c>
-      <c r="I29">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1029</v>
       </c>
@@ -4012,20 +3653,8 @@
       <c r="E30">
         <v>0.47731092400000003</v>
       </c>
-      <c r="F30">
-        <v>0.5</v>
-      </c>
-      <c r="G30">
-        <v>0.5</v>
-      </c>
-      <c r="H30">
-        <v>0.5</v>
-      </c>
-      <c r="I30">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1030</v>
       </c>
@@ -4041,20 +3670,8 @@
       <c r="E31">
         <v>0.50997426000000001</v>
       </c>
-      <c r="F31">
-        <v>0.5</v>
-      </c>
-      <c r="G31">
-        <v>0.5</v>
-      </c>
-      <c r="H31">
-        <v>0.5</v>
-      </c>
-      <c r="I31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1031</v>
       </c>
@@ -4070,20 +3687,8 @@
       <c r="E32">
         <v>0.38105107999999999</v>
       </c>
-      <c r="F32">
-        <v>0.5</v>
-      </c>
-      <c r="G32">
-        <v>0.5</v>
-      </c>
-      <c r="H32">
-        <v>0.5</v>
-      </c>
-      <c r="I32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1032</v>
       </c>
@@ -4099,20 +3704,8 @@
       <c r="E33">
         <v>0.58117647100000003</v>
       </c>
-      <c r="F33">
-        <v>0.5</v>
-      </c>
-      <c r="G33">
-        <v>0.5</v>
-      </c>
-      <c r="H33">
-        <v>0.5</v>
-      </c>
-      <c r="I33">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1033</v>
       </c>
@@ -4128,20 +3721,8 @@
       <c r="E34">
         <v>0.54411497200000003</v>
       </c>
-      <c r="F34">
-        <v>0.5</v>
-      </c>
-      <c r="G34">
-        <v>0.5</v>
-      </c>
-      <c r="H34">
-        <v>0.5</v>
-      </c>
-      <c r="I34">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1034</v>
       </c>
@@ -4157,20 +3738,8 @@
       <c r="E35">
         <v>0.58825514700000003</v>
       </c>
-      <c r="F35">
-        <v>0.5</v>
-      </c>
-      <c r="G35">
-        <v>0.5</v>
-      </c>
-      <c r="H35">
-        <v>0.5</v>
-      </c>
-      <c r="I35">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1035</v>
       </c>
@@ -4186,20 +3755,8 @@
       <c r="E36">
         <v>0.64577918999999995</v>
       </c>
-      <c r="F36">
-        <v>0.5</v>
-      </c>
-      <c r="G36">
-        <v>0.5</v>
-      </c>
-      <c r="H36">
-        <v>0.5</v>
-      </c>
-      <c r="I36">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1059</v>
       </c>
@@ -4215,20 +3772,8 @@
       <c r="E37">
         <v>0.451962111</v>
       </c>
-      <c r="F37">
-        <v>0.5</v>
-      </c>
-      <c r="G37">
-        <v>0.5</v>
-      </c>
-      <c r="H37">
-        <v>0.5</v>
-      </c>
-      <c r="I37">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1060</v>
       </c>
@@ -4244,20 +3789,8 @@
       <c r="E38">
         <v>0.54591739100000003</v>
       </c>
-      <c r="F38">
-        <v>0.5</v>
-      </c>
-      <c r="G38">
-        <v>0.5</v>
-      </c>
-      <c r="H38">
-        <v>0.5</v>
-      </c>
-      <c r="I38">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1061</v>
       </c>
@@ -4273,20 +3806,8 @@
       <c r="E39">
         <v>0.51635750400000002</v>
       </c>
-      <c r="F39">
-        <v>0.5</v>
-      </c>
-      <c r="G39">
-        <v>0.5</v>
-      </c>
-      <c r="H39">
-        <v>0.5</v>
-      </c>
-      <c r="I39">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1062</v>
       </c>
@@ -4302,20 +3823,8 @@
       <c r="E40">
         <v>0.511530398</v>
       </c>
-      <c r="F40">
-        <v>0.5</v>
-      </c>
-      <c r="G40">
-        <v>0.5</v>
-      </c>
-      <c r="H40">
-        <v>0.5</v>
-      </c>
-      <c r="I40">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1063</v>
       </c>
@@ -4331,20 +3840,8 @@
       <c r="E41">
         <v>0.38816362100000001</v>
       </c>
-      <c r="F41">
-        <v>0.5</v>
-      </c>
-      <c r="G41">
-        <v>0.5</v>
-      </c>
-      <c r="H41">
-        <v>0.5</v>
-      </c>
-      <c r="I41">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1064</v>
       </c>
@@ -4360,20 +3857,8 @@
       <c r="E42">
         <v>0.24470850399999999</v>
       </c>
-      <c r="F42">
-        <v>0.5</v>
-      </c>
-      <c r="G42">
-        <v>0.5</v>
-      </c>
-      <c r="H42">
-        <v>0.5</v>
-      </c>
-      <c r="I42">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1065</v>
       </c>
@@ -4389,20 +3874,8 @@
       <c r="E43">
         <v>0.48951049000000002</v>
       </c>
-      <c r="F43">
-        <v>0.5</v>
-      </c>
-      <c r="G43">
-        <v>0.5</v>
-      </c>
-      <c r="H43">
-        <v>0.5</v>
-      </c>
-      <c r="I43">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1066</v>
       </c>
@@ -4418,20 +3891,8 @@
       <c r="E44">
         <v>0.25768321500000002</v>
       </c>
-      <c r="F44">
-        <v>0.5</v>
-      </c>
-      <c r="G44">
-        <v>0.5</v>
-      </c>
-      <c r="H44">
-        <v>0.5</v>
-      </c>
-      <c r="I44">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1067</v>
       </c>
@@ -4447,20 +3908,8 @@
       <c r="E45">
         <v>0.494111623</v>
       </c>
-      <c r="F45">
-        <v>0.5</v>
-      </c>
-      <c r="G45">
-        <v>0.5</v>
-      </c>
-      <c r="H45">
-        <v>0.5</v>
-      </c>
-      <c r="I45">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1068</v>
       </c>
@@ -4476,20 +3925,8 @@
       <c r="E46">
         <v>0.52259075499999996</v>
       </c>
-      <c r="F46">
-        <v>0.5</v>
-      </c>
-      <c r="G46">
-        <v>0.5</v>
-      </c>
-      <c r="H46">
-        <v>0.5</v>
-      </c>
-      <c r="I46">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1069</v>
       </c>
@@ -4505,20 +3942,8 @@
       <c r="E47">
         <v>0.490296595</v>
       </c>
-      <c r="F47">
-        <v>0.5</v>
-      </c>
-      <c r="G47">
-        <v>0.5</v>
-      </c>
-      <c r="H47">
-        <v>0.5</v>
-      </c>
-      <c r="I47">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1070</v>
       </c>
@@ -4534,20 +3959,8 @@
       <c r="E48">
         <v>0.53155506699999999</v>
       </c>
-      <c r="F48">
-        <v>0.5</v>
-      </c>
-      <c r="G48">
-        <v>0.5</v>
-      </c>
-      <c r="H48">
-        <v>0.5</v>
-      </c>
-      <c r="I48">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1071</v>
       </c>
@@ -4563,20 +3976,8 @@
       <c r="E49">
         <v>0.51688048600000003</v>
       </c>
-      <c r="F49">
-        <v>0.5</v>
-      </c>
-      <c r="G49">
-        <v>0.5</v>
-      </c>
-      <c r="H49">
-        <v>0.5</v>
-      </c>
-      <c r="I49">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1072</v>
       </c>
@@ -4592,20 +3993,8 @@
       <c r="E50">
         <v>0.427995972</v>
       </c>
-      <c r="F50">
-        <v>0.5</v>
-      </c>
-      <c r="G50">
-        <v>0.5</v>
-      </c>
-      <c r="H50">
-        <v>0.5</v>
-      </c>
-      <c r="I50">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1073</v>
       </c>
@@ -4621,20 +4010,8 @@
       <c r="E51">
         <v>0.54840494200000001</v>
       </c>
-      <c r="F51">
-        <v>0.5</v>
-      </c>
-      <c r="G51">
-        <v>0.5</v>
-      </c>
-      <c r="H51">
-        <v>0.5</v>
-      </c>
-      <c r="I51">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1074</v>
       </c>
@@ -4650,20 +4027,8 @@
       <c r="E52">
         <v>0.50571836999999997</v>
       </c>
-      <c r="F52">
-        <v>0.5</v>
-      </c>
-      <c r="G52">
-        <v>0.5</v>
-      </c>
-      <c r="H52">
-        <v>0.5</v>
-      </c>
-      <c r="I52">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1075</v>
       </c>
@@ -4679,20 +4044,8 @@
       <c r="E53">
         <v>0.57261098600000004</v>
       </c>
-      <c r="F53">
-        <v>0.5</v>
-      </c>
-      <c r="G53">
-        <v>0.5</v>
-      </c>
-      <c r="H53">
-        <v>0.5</v>
-      </c>
-      <c r="I53">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1076</v>
       </c>
@@ -4708,20 +4061,8 @@
       <c r="E54">
         <v>0.53573238700000003</v>
       </c>
-      <c r="F54">
-        <v>0.5</v>
-      </c>
-      <c r="G54">
-        <v>0.5</v>
-      </c>
-      <c r="H54">
-        <v>0.5</v>
-      </c>
-      <c r="I54">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1077</v>
       </c>
@@ -4737,20 +4078,8 @@
       <c r="E55">
         <v>0.40434666000000002</v>
       </c>
-      <c r="F55">
-        <v>0.5</v>
-      </c>
-      <c r="G55">
-        <v>0.5</v>
-      </c>
-      <c r="H55">
-        <v>0.5</v>
-      </c>
-      <c r="I55">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1078</v>
       </c>
@@ -4766,20 +4095,8 @@
       <c r="E56">
         <v>0.395995551</v>
       </c>
-      <c r="F56">
-        <v>0.5</v>
-      </c>
-      <c r="G56">
-        <v>0.5</v>
-      </c>
-      <c r="H56">
-        <v>0.5</v>
-      </c>
-      <c r="I56">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1079</v>
       </c>
@@ -4795,20 +4112,8 @@
       <c r="E57">
         <v>0.460748349</v>
       </c>
-      <c r="F57">
-        <v>0.5</v>
-      </c>
-      <c r="G57">
-        <v>0.5</v>
-      </c>
-      <c r="H57">
-        <v>0.5</v>
-      </c>
-      <c r="I57">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1080</v>
       </c>
@@ -4824,20 +4129,8 @@
       <c r="E58">
         <v>0.41122484999999998</v>
       </c>
-      <c r="F58">
-        <v>0.5</v>
-      </c>
-      <c r="G58">
-        <v>0.5</v>
-      </c>
-      <c r="H58">
-        <v>0.5</v>
-      </c>
-      <c r="I58">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1081</v>
       </c>
@@ -4853,20 +4146,8 @@
       <c r="E59">
         <v>0.58149779700000004</v>
       </c>
-      <c r="F59">
-        <v>0.5</v>
-      </c>
-      <c r="G59">
-        <v>0.5</v>
-      </c>
-      <c r="H59">
-        <v>0.5</v>
-      </c>
-      <c r="I59">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1082</v>
       </c>
@@ -4882,20 +4163,8 @@
       <c r="E60">
         <v>0.56561086000000005</v>
       </c>
-      <c r="F60">
-        <v>0.5</v>
-      </c>
-      <c r="G60">
-        <v>0.5</v>
-      </c>
-      <c r="H60">
-        <v>0.5</v>
-      </c>
-      <c r="I60">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1083</v>
       </c>
@@ -4911,20 +4180,8 @@
       <c r="E61">
         <v>0.24127691200000001</v>
       </c>
-      <c r="F61">
-        <v>0.5</v>
-      </c>
-      <c r="G61">
-        <v>0.5</v>
-      </c>
-      <c r="H61">
-        <v>0.5</v>
-      </c>
-      <c r="I61">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1084</v>
       </c>
@@ -4940,20 +4197,8 @@
       <c r="E62">
         <v>0.36368421099999998</v>
       </c>
-      <c r="F62">
-        <v>0.5</v>
-      </c>
-      <c r="G62">
-        <v>0.5</v>
-      </c>
-      <c r="H62">
-        <v>0.5</v>
-      </c>
-      <c r="I62">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1085</v>
       </c>
@@ -4969,20 +4214,8 @@
       <c r="E63">
         <v>0.43116426299999999</v>
       </c>
-      <c r="F63">
-        <v>0.5</v>
-      </c>
-      <c r="G63">
-        <v>0.5</v>
-      </c>
-      <c r="H63">
-        <v>0.5</v>
-      </c>
-      <c r="I63">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1086</v>
       </c>
@@ -4998,20 +4231,8 @@
       <c r="E64">
         <v>0.20065390399999999</v>
       </c>
-      <c r="F64">
-        <v>0.5</v>
-      </c>
-      <c r="G64">
-        <v>0.5</v>
-      </c>
-      <c r="H64">
-        <v>0.5</v>
-      </c>
-      <c r="I64">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1087</v>
       </c>
@@ -5027,20 +4248,8 @@
       <c r="E65">
         <v>0.42688882500000003</v>
       </c>
-      <c r="F65">
-        <v>0.5</v>
-      </c>
-      <c r="G65">
-        <v>0.5</v>
-      </c>
-      <c r="H65">
-        <v>0.5</v>
-      </c>
-      <c r="I65">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1089</v>
       </c>
@@ -5056,20 +4265,8 @@
       <c r="E66">
         <v>0.66843501299999997</v>
       </c>
-      <c r="F66">
-        <v>0.5</v>
-      </c>
-      <c r="G66">
-        <v>0.5</v>
-      </c>
-      <c r="H66">
-        <v>0.5</v>
-      </c>
-      <c r="I66">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1090</v>
       </c>
@@ -5085,20 +4282,8 @@
       <c r="E67">
         <v>0.37324602400000001</v>
       </c>
-      <c r="F67">
-        <v>0.5</v>
-      </c>
-      <c r="G67">
-        <v>0.5</v>
-      </c>
-      <c r="H67">
-        <v>0.5</v>
-      </c>
-      <c r="I67">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1091</v>
       </c>
@@ -5114,20 +4299,8 @@
       <c r="E68">
         <v>0.62905263199999994</v>
       </c>
-      <c r="F68">
-        <v>0.5</v>
-      </c>
-      <c r="G68">
-        <v>0.5</v>
-      </c>
-      <c r="H68">
-        <v>0.5</v>
-      </c>
-      <c r="I68">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1092</v>
       </c>
@@ -5143,20 +4316,8 @@
       <c r="E69">
         <v>0.58413597699999997</v>
       </c>
-      <c r="F69">
-        <v>0.5</v>
-      </c>
-      <c r="G69">
-        <v>0.5</v>
-      </c>
-      <c r="H69">
-        <v>0.5</v>
-      </c>
-      <c r="I69">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1093</v>
       </c>
@@ -5172,20 +4333,8 @@
       <c r="E70">
         <v>0.42566983600000002</v>
       </c>
-      <c r="F70">
-        <v>0.5</v>
-      </c>
-      <c r="G70">
-        <v>0.5</v>
-      </c>
-      <c r="H70">
-        <v>0.5</v>
-      </c>
-      <c r="I70">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1117</v>
       </c>
@@ -5201,20 +4350,8 @@
       <c r="E71">
         <v>0.55233681000000001</v>
       </c>
-      <c r="F71">
-        <v>0.5</v>
-      </c>
-      <c r="G71">
-        <v>0.5</v>
-      </c>
-      <c r="H71">
-        <v>0.5</v>
-      </c>
-      <c r="I71">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1118</v>
       </c>
@@ -5230,20 +4367,8 @@
       <c r="E72">
         <v>0.54052149400000005</v>
       </c>
-      <c r="F72">
-        <v>0.5</v>
-      </c>
-      <c r="G72">
-        <v>0.5</v>
-      </c>
-      <c r="H72">
-        <v>0.5</v>
-      </c>
-      <c r="I72">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1119</v>
       </c>
@@ -5259,20 +4384,8 @@
       <c r="E73">
         <v>0.470749902</v>
       </c>
-      <c r="F73">
-        <v>0.5</v>
-      </c>
-      <c r="G73">
-        <v>0.5</v>
-      </c>
-      <c r="H73">
-        <v>0.5</v>
-      </c>
-      <c r="I73">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1120</v>
       </c>
@@ -5288,20 +4401,8 @@
       <c r="E74">
         <v>0.484161126</v>
       </c>
-      <c r="F74">
-        <v>0.5</v>
-      </c>
-      <c r="G74">
-        <v>0.5</v>
-      </c>
-      <c r="H74">
-        <v>0.5</v>
-      </c>
-      <c r="I74">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1121</v>
       </c>
@@ -5317,20 +4418,8 @@
       <c r="E75">
         <v>0.50780100100000003</v>
       </c>
-      <c r="F75">
-        <v>0.5</v>
-      </c>
-      <c r="G75">
-        <v>0.5</v>
-      </c>
-      <c r="H75">
-        <v>0.5</v>
-      </c>
-      <c r="I75">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1122</v>
       </c>
@@ -5346,20 +4435,8 @@
       <c r="E76">
         <v>0.39940652799999998</v>
       </c>
-      <c r="F76">
-        <v>0.5</v>
-      </c>
-      <c r="G76">
-        <v>0.5</v>
-      </c>
-      <c r="H76">
-        <v>0.5</v>
-      </c>
-      <c r="I76">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1123</v>
       </c>
@@ -5375,20 +4452,8 @@
       <c r="E77">
         <v>0.48648073200000003</v>
       </c>
-      <c r="F77">
-        <v>0.5</v>
-      </c>
-      <c r="G77">
-        <v>0.5</v>
-      </c>
-      <c r="H77">
-        <v>0.5</v>
-      </c>
-      <c r="I77">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1124</v>
       </c>
@@ -5404,20 +4469,8 @@
       <c r="E78">
         <v>0.51240931700000003</v>
       </c>
-      <c r="F78">
-        <v>0.5</v>
-      </c>
-      <c r="G78">
-        <v>0.5</v>
-      </c>
-      <c r="H78">
-        <v>0.5</v>
-      </c>
-      <c r="I78">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1125</v>
       </c>
@@ -5433,20 +4486,8 @@
       <c r="E79">
         <v>0.44718693300000001</v>
       </c>
-      <c r="F79">
-        <v>0.5</v>
-      </c>
-      <c r="G79">
-        <v>0.5</v>
-      </c>
-      <c r="H79">
-        <v>0.5</v>
-      </c>
-      <c r="I79">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1127</v>
       </c>
@@ -5462,20 +4503,8 @@
       <c r="E80">
         <v>0.47092245999999999</v>
       </c>
-      <c r="F80">
-        <v>0.5</v>
-      </c>
-      <c r="G80">
-        <v>0.5</v>
-      </c>
-      <c r="H80">
-        <v>0.5</v>
-      </c>
-      <c r="I80">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1131</v>
       </c>
@@ -5491,20 +4520,8 @@
       <c r="E81">
         <v>0.62020517399999997</v>
       </c>
-      <c r="F81">
-        <v>0.5</v>
-      </c>
-      <c r="G81">
-        <v>0.5</v>
-      </c>
-      <c r="H81">
-        <v>0.5</v>
-      </c>
-      <c r="I81">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1132</v>
       </c>
@@ -5520,20 +4537,8 @@
       <c r="E82">
         <v>0.54365541299999998</v>
       </c>
-      <c r="F82">
-        <v>0.5</v>
-      </c>
-      <c r="G82">
-        <v>0.5</v>
-      </c>
-      <c r="H82">
-        <v>0.5</v>
-      </c>
-      <c r="I82">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1133</v>
       </c>
@@ -5549,20 +4554,8 @@
       <c r="E83">
         <v>0.64806135499999995</v>
       </c>
-      <c r="F83">
-        <v>0.5</v>
-      </c>
-      <c r="G83">
-        <v>0.5</v>
-      </c>
-      <c r="H83">
-        <v>0.5</v>
-      </c>
-      <c r="I83">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1134</v>
       </c>
@@ -5578,20 +4571,8 @@
       <c r="E84">
         <v>0.53705118399999996</v>
       </c>
-      <c r="F84">
-        <v>0.5</v>
-      </c>
-      <c r="G84">
-        <v>0.5</v>
-      </c>
-      <c r="H84">
-        <v>0.5</v>
-      </c>
-      <c r="I84">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1135</v>
       </c>
@@ -5607,20 +4588,8 @@
       <c r="E85">
         <v>0.60526315799999997</v>
       </c>
-      <c r="F85">
-        <v>0.5</v>
-      </c>
-      <c r="G85">
-        <v>0.5</v>
-      </c>
-      <c r="H85">
-        <v>0.5</v>
-      </c>
-      <c r="I85">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1136</v>
       </c>
@@ -5636,20 +4605,8 @@
       <c r="E86">
         <v>0.586770982</v>
       </c>
-      <c r="F86">
-        <v>0.5</v>
-      </c>
-      <c r="G86">
-        <v>0.5</v>
-      </c>
-      <c r="H86">
-        <v>0.5</v>
-      </c>
-      <c r="I86">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1137</v>
       </c>
@@ -5665,20 +4622,8 @@
       <c r="E87">
         <v>0.51853568100000003</v>
       </c>
-      <c r="F87">
-        <v>0.5</v>
-      </c>
-      <c r="G87">
-        <v>0.5</v>
-      </c>
-      <c r="H87">
-        <v>0.5</v>
-      </c>
-      <c r="I87">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1138</v>
       </c>
@@ -5694,20 +4639,8 @@
       <c r="E88">
         <v>0.56959118099999995</v>
       </c>
-      <c r="F88">
-        <v>0.5</v>
-      </c>
-      <c r="G88">
-        <v>0.5</v>
-      </c>
-      <c r="H88">
-        <v>0.5</v>
-      </c>
-      <c r="I88">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1139</v>
       </c>
@@ -5723,20 +4656,8 @@
       <c r="E89">
         <v>0.42355008799999999</v>
       </c>
-      <c r="F89">
-        <v>0.5</v>
-      </c>
-      <c r="G89">
-        <v>0.5</v>
-      </c>
-      <c r="H89">
-        <v>0.5</v>
-      </c>
-      <c r="I89">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1140</v>
       </c>
@@ -5752,20 +4673,8 @@
       <c r="E90">
         <v>0.33272394900000002</v>
       </c>
-      <c r="F90">
-        <v>0.5</v>
-      </c>
-      <c r="G90">
-        <v>0.5</v>
-      </c>
-      <c r="H90">
-        <v>0.5</v>
-      </c>
-      <c r="I90">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1142</v>
       </c>
@@ -5781,20 +4690,8 @@
       <c r="E91">
         <v>0.41655520899999998</v>
       </c>
-      <c r="F91">
-        <v>0.5</v>
-      </c>
-      <c r="G91">
-        <v>0.5</v>
-      </c>
-      <c r="H91">
-        <v>0.5</v>
-      </c>
-      <c r="I91">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1143</v>
       </c>
@@ -5810,20 +4707,8 @@
       <c r="E92">
         <v>0.41184971100000001</v>
       </c>
-      <c r="F92">
-        <v>0.5</v>
-      </c>
-      <c r="G92">
-        <v>0.5</v>
-      </c>
-      <c r="H92">
-        <v>0.5</v>
-      </c>
-      <c r="I92">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1144</v>
       </c>
@@ -5839,20 +4724,8 @@
       <c r="E93">
         <v>0.57738340899999996</v>
       </c>
-      <c r="F93">
-        <v>0.5</v>
-      </c>
-      <c r="G93">
-        <v>0.5</v>
-      </c>
-      <c r="H93">
-        <v>0.5</v>
-      </c>
-      <c r="I93">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1145</v>
       </c>
@@ -5868,20 +4741,8 @@
       <c r="E94">
         <v>0.58068149800000002</v>
       </c>
-      <c r="F94">
-        <v>0.5</v>
-      </c>
-      <c r="G94">
-        <v>0.5</v>
-      </c>
-      <c r="H94">
-        <v>0.5</v>
-      </c>
-      <c r="I94">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1146</v>
       </c>
@@ -5897,20 +4758,8 @@
       <c r="E95">
         <v>0.55821474800000004</v>
       </c>
-      <c r="F95">
-        <v>0.5</v>
-      </c>
-      <c r="G95">
-        <v>0.5</v>
-      </c>
-      <c r="H95">
-        <v>0.5</v>
-      </c>
-      <c r="I95">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1147</v>
       </c>
@@ -5926,20 +4775,8 @@
       <c r="E96">
         <v>0.42578644199999999</v>
       </c>
-      <c r="F96">
-        <v>0.5</v>
-      </c>
-      <c r="G96">
-        <v>0.5</v>
-      </c>
-      <c r="H96">
-        <v>0.5</v>
-      </c>
-      <c r="I96">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1148</v>
       </c>
@@ -5955,20 +4792,8 @@
       <c r="E97">
         <v>0.45814978000000001</v>
       </c>
-      <c r="F97">
-        <v>0.5</v>
-      </c>
-      <c r="G97">
-        <v>0.5</v>
-      </c>
-      <c r="H97">
-        <v>0.5</v>
-      </c>
-      <c r="I97">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1149</v>
       </c>
@@ -5984,20 +4809,8 @@
       <c r="E98">
         <v>0.53685092099999998</v>
       </c>
-      <c r="F98">
-        <v>0.5</v>
-      </c>
-      <c r="G98">
-        <v>0.5</v>
-      </c>
-      <c r="H98">
-        <v>0.5</v>
-      </c>
-      <c r="I98">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1150</v>
       </c>
@@ -6013,20 +4826,8 @@
       <c r="E99">
         <v>0.46289169899999999</v>
       </c>
-      <c r="F99">
-        <v>0.5</v>
-      </c>
-      <c r="G99">
-        <v>0.5</v>
-      </c>
-      <c r="H99">
-        <v>0.5</v>
-      </c>
-      <c r="I99">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1151</v>
       </c>
@@ -6042,20 +4843,8 @@
       <c r="E100">
         <v>0.50779510000000005</v>
       </c>
-      <c r="F100">
-        <v>0.5</v>
-      </c>
-      <c r="G100">
-        <v>0.5</v>
-      </c>
-      <c r="H100">
-        <v>0.5</v>
-      </c>
-      <c r="I100">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1152</v>
       </c>
@@ -6071,20 +4860,8 @@
       <c r="E101">
         <v>0.31944444399999999</v>
       </c>
-      <c r="F101">
-        <v>0.5</v>
-      </c>
-      <c r="G101">
-        <v>0.5</v>
-      </c>
-      <c r="H101">
-        <v>0.5</v>
-      </c>
-      <c r="I101">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1153</v>
       </c>
@@ -6100,20 +4877,8 @@
       <c r="E102">
         <v>0.52434077099999998</v>
       </c>
-      <c r="F102">
-        <v>0.5</v>
-      </c>
-      <c r="G102">
-        <v>0.5</v>
-      </c>
-      <c r="H102">
-        <v>0.5</v>
-      </c>
-      <c r="I102">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1154</v>
       </c>
@@ -6129,20 +4894,8 @@
       <c r="E103">
         <v>0.52030947800000005</v>
       </c>
-      <c r="F103">
-        <v>0.5</v>
-      </c>
-      <c r="G103">
-        <v>0.5</v>
-      </c>
-      <c r="H103">
-        <v>0.5</v>
-      </c>
-      <c r="I103">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1155</v>
       </c>
@@ -6158,20 +4911,8 @@
       <c r="E104">
         <v>0.37134909599999999</v>
       </c>
-      <c r="F104">
-        <v>0.5</v>
-      </c>
-      <c r="G104">
-        <v>0.5</v>
-      </c>
-      <c r="H104">
-        <v>0.5</v>
-      </c>
-      <c r="I104">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>1156</v>
       </c>
@@ -6187,20 +4928,8 @@
       <c r="E105">
         <v>0.58318840599999999</v>
       </c>
-      <c r="F105">
-        <v>0.5</v>
-      </c>
-      <c r="G105">
-        <v>0.5</v>
-      </c>
-      <c r="H105">
-        <v>0.5</v>
-      </c>
-      <c r="I105">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1157</v>
       </c>
@@ -6216,20 +4945,8 @@
       <c r="E106">
         <v>0.46854182100000002</v>
       </c>
-      <c r="F106">
-        <v>0.5</v>
-      </c>
-      <c r="G106">
-        <v>0.5</v>
-      </c>
-      <c r="H106">
-        <v>0.5</v>
-      </c>
-      <c r="I106">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>1158</v>
       </c>
@@ -6245,20 +4962,8 @@
       <c r="E107">
         <v>0.45063103199999999</v>
       </c>
-      <c r="F107">
-        <v>0.5</v>
-      </c>
-      <c r="G107">
-        <v>0.5</v>
-      </c>
-      <c r="H107">
-        <v>0.5</v>
-      </c>
-      <c r="I107">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1160</v>
       </c>
@@ -6274,20 +4979,8 @@
       <c r="E108">
         <v>0.60081674299999999</v>
       </c>
-      <c r="F108">
-        <v>0.5</v>
-      </c>
-      <c r="G108">
-        <v>0.5</v>
-      </c>
-      <c r="H108">
-        <v>0.5</v>
-      </c>
-      <c r="I108">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>1161</v>
       </c>
@@ -6303,20 +4996,8 @@
       <c r="E109">
         <v>0.55438251900000002</v>
       </c>
-      <c r="F109">
-        <v>0.5</v>
-      </c>
-      <c r="G109">
-        <v>0.5</v>
-      </c>
-      <c r="H109">
-        <v>0.5</v>
-      </c>
-      <c r="I109">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1162</v>
       </c>
@@ -6332,20 +5013,8 @@
       <c r="E110">
         <v>0.46851956900000002</v>
       </c>
-      <c r="F110">
-        <v>0.5</v>
-      </c>
-      <c r="G110">
-        <v>0.5</v>
-      </c>
-      <c r="H110">
-        <v>0.5</v>
-      </c>
-      <c r="I110">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>1163</v>
       </c>
@@ -6361,20 +5030,8 @@
       <c r="E111">
         <v>0.54359925799999997</v>
       </c>
-      <c r="F111">
-        <v>0.5</v>
-      </c>
-      <c r="G111">
-        <v>0.5</v>
-      </c>
-      <c r="H111">
-        <v>0.5</v>
-      </c>
-      <c r="I111">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>1164</v>
       </c>
@@ -6390,20 +5047,8 @@
       <c r="E112">
         <v>0.49546279500000001</v>
       </c>
-      <c r="F112">
-        <v>0.5</v>
-      </c>
-      <c r="G112">
-        <v>0.5</v>
-      </c>
-      <c r="H112">
-        <v>0.5</v>
-      </c>
-      <c r="I112">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1165</v>
       </c>
@@ -6418,18 +5063,6 @@
       </c>
       <c r="E113">
         <v>0.45950864400000002</v>
-      </c>
-      <c r="F113">
-        <v>0.5</v>
-      </c>
-      <c r="G113">
-        <v>0.5</v>
-      </c>
-      <c r="H113">
-        <v>0.5</v>
-      </c>
-      <c r="I113">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -6453,15 +5086,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B2">
         <f>(5/9)</f>
@@ -6470,7 +5103,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B3">
         <f>(6/9)</f>
@@ -6479,7 +5112,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B4">
         <f>(4/9)</f>
@@ -6488,7 +5121,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B5">
         <f>(6/9)</f>
@@ -6504,7 +5137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -6516,15 +5149,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <v>0.592592593</v>
@@ -6532,7 +5165,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B3">
         <v>0.592592593</v>
@@ -6540,7 +5173,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B4">
         <v>0.592592593</v>
@@ -6548,7 +5181,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B5">
         <v>0.592592593</v>
@@ -6556,7 +5189,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B6">
         <v>0.592592593</v>
@@ -6564,7 +5197,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B7">
         <v>0.592592593</v>
@@ -6591,15 +5224,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B2">
         <v>0.53012048199999995</v>
@@ -6607,7 +5240,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>0.50602409599999998</v>
@@ -6615,7 +5248,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B4">
         <v>0.53012048000000001</v>
@@ -6623,7 +5256,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B5">
         <v>0.53012482000000005</v>
@@ -6631,7 +5264,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B6">
         <v>0.53012049999999999</v>
@@ -6639,7 +5272,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B7">
         <v>0.54216867499999999</v>
@@ -6666,15 +5299,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B2">
         <v>0.4</v>
@@ -6682,7 +5315,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>0.36</v>
@@ -6690,7 +5323,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B4">
         <v>0.4</v>
@@ -6698,7 +5331,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B5">
         <v>0.4</v>
@@ -6706,7 +5339,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B6">
         <v>0.4</v>
@@ -6734,18 +5367,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B2">
         <v>0.592592593</v>
@@ -6756,7 +5389,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B3">
         <v>0.52811244999999996</v>
@@ -6767,7 +5400,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B4">
         <v>0.39200000000000002</v>

</xml_diff>